<commit_message>
coordinates; pvrp format; scheduling
coordinates now cleaner

pvrp format still has scheduling problems

scheduling move to pvrp format on its way
</commit_message>
<xml_diff>
--- a/data/TR/results/All_Long_Solutions.xlsx
+++ b/data/TR/results/All_Long_Solutions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="32">
   <si>
     <t>Filename</t>
   </si>
@@ -115,43 +115,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="13">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <i val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <i val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -224,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
@@ -246,26 +216,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -278,16 +228,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.54296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.2890625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.90625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.7734375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.35546875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.9921875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.39453125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.9140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.87109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="21">
+      <c r="A1" t="s" s="9">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -295,7 +245,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="21">
+      <c r="A2" t="s" s="9">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -303,7 +253,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="21">
+      <c r="A3" t="s" s="9">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -311,7 +261,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="21">
+      <c r="A4" t="s" s="9">
         <v>6</v>
       </c>
       <c r="B4" t="n">
@@ -319,22 +269,22 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="21">
+      <c r="A5" t="s" s="9">
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>25.0</v>
+        <v>15.0</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="21">
+      <c r="A6" t="s" s="9">
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>25.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="7">
@@ -353,17 +303,17 @@
         <v>12</v>
       </c>
       <c r="B8" t="n">
-        <v>2277.0</v>
+        <v>2229.0</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="19">
+      <c r="A9" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="B9" t="s" s="19">
+      <c r="B9" t="s" s="7">
         <v>15</v>
       </c>
     </row>
@@ -372,19 +322,19 @@
     <row r="12"/>
     <row r="13"/>
     <row r="14">
-      <c r="A14" t="s" s="19">
+      <c r="A14" t="s" s="7">
         <v>16</v>
       </c>
       <c r="B14" t="n">
         <v>-1.0</v>
       </c>
-      <c r="C14" t="s" s="19">
+      <c r="C14" t="s" s="7">
         <v>17</v>
       </c>
       <c r="D14" t="n">
         <v>-80.046878</v>
       </c>
-      <c r="E14" t="s" s="19">
+      <c r="E14" t="s" s="7">
         <v>18</v>
       </c>
       <c r="F14" t="n">
@@ -392,37 +342,37 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="19">
+      <c r="A15" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="B15" t="n" s="19">
+      <c r="B15" t="n" s="7">
         <v>0.0</v>
       </c>
-      <c r="C15" t="s" s="19">
+      <c r="C15" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="D15" t="n" s="20">
+      <c r="D15" t="n" s="8">
         <v>-1.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s" s="19">
+      <c r="A16" t="s" s="7">
         <v>21</v>
       </c>
-      <c r="B16" t="n" s="20">
-        <v>6.831668376922607</v>
-      </c>
-      <c r="C16" t="s" s="19">
+      <c r="B16" t="n" s="8">
+        <v>4.249732494354248</v>
+      </c>
+      <c r="C16" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="D16" t="n" s="20">
-        <v>450.0</v>
-      </c>
-      <c r="E16" t="s" s="19">
+      <c r="D16" t="n" s="8">
+        <v>437.0</v>
+      </c>
+      <c r="E16" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="F16" t="n" s="20">
-        <v>6.831668376922607</v>
+      <c r="F16" t="n" s="8">
+        <v>4.249732494354248</v>
       </c>
     </row>
     <row r="17"/>
@@ -474,13 +424,13 @@
         <v>2.0</v>
       </c>
       <c r="C20" t="n">
-        <v>0.04200505092740059</v>
+        <v>0.026129815727472305</v>
       </c>
       <c r="D20" t="n">
         <v>262.0077728246056</v>
       </c>
       <c r="E20" t="n">
-        <v>0.04200505092740059</v>
+        <v>0.026129815727472305</v>
       </c>
       <c r="F20" t="n">
         <v>1.0</v>
@@ -494,13 +444,13 @@
         <v>1.0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4929746091365814</v>
+        <v>0.30666160583496094</v>
       </c>
       <c r="D21" t="n">
         <v>261.8645538790942</v>
       </c>
       <c r="E21" t="n">
-        <v>0.45410019159317017</v>
+        <v>0.2824792265892029</v>
       </c>
       <c r="F21" t="n">
         <v>4.0</v>
@@ -514,13 +464,13 @@
         <v>1.0</v>
       </c>
       <c r="C22" t="n">
-        <v>1.1177265644073486</v>
+        <v>0.6952970623970032</v>
       </c>
       <c r="D22" t="n">
         <v>261.8127084459809</v>
       </c>
       <c r="E22" t="n">
-        <v>0.6735409498214722</v>
+        <v>0.4189853370189667</v>
       </c>
       <c r="F22" t="n">
         <v>1.0</v>
@@ -534,13 +484,13 @@
         <v>2.0</v>
       </c>
       <c r="C23" t="n">
-        <v>1.279657006263733</v>
+        <v>0.7960281372070312</v>
       </c>
       <c r="D23" t="n">
         <v>261.74558639022837</v>
       </c>
       <c r="E23" t="n">
-        <v>0.17964953184127808</v>
+        <v>0.1117534413933754</v>
       </c>
       <c r="F23" t="n">
         <v>1.0</v>
@@ -554,13 +504,13 @@
         <v>2.0</v>
       </c>
       <c r="C24" t="n">
-        <v>1.2688837051391602</v>
+        <v>0.7893264293670654</v>
       </c>
       <c r="D24" t="n">
         <v>261.734512161128</v>
       </c>
       <c r="E24" t="n">
-        <v>0.033480454236269</v>
+        <v>0.020826974883675575</v>
       </c>
       <c r="F24" t="n">
         <v>1.0</v>
@@ -574,13 +524,13 @@
         <v>1.0</v>
       </c>
       <c r="C25" t="n">
-        <v>1.5365809202194214</v>
+        <v>0.9558511972427368</v>
       </c>
       <c r="D25" t="n">
         <v>261.4050595755135</v>
       </c>
       <c r="E25" t="n">
-        <v>0.740107536315918</v>
+        <v>0.4603939950466156</v>
       </c>
       <c r="F25" t="n">
         <v>1.0</v>
@@ -594,13 +544,13 @@
         <v>2.0</v>
       </c>
       <c r="C26" t="n">
-        <v>1.244834303855896</v>
+        <v>0.7743661999702454</v>
       </c>
       <c r="D26" t="n">
         <v>261.5087901924117</v>
       </c>
       <c r="E26" t="n">
-        <v>0.29834985733032227</v>
+        <v>0.18559260666370392</v>
       </c>
       <c r="F26" t="n">
         <v>1.0</v>
@@ -614,13 +564,13 @@
         <v>2.0</v>
       </c>
       <c r="C27" t="n">
-        <v>1.2301167249679565</v>
+        <v>0.7652108669281006</v>
       </c>
       <c r="D27" t="n">
         <v>261.4937537372069</v>
       </c>
       <c r="E27" t="n">
-        <v>0.09499038755893707</v>
+        <v>0.05909006670117378</v>
       </c>
       <c r="F27" t="n">
         <v>1.0</v>
@@ -634,13 +584,13 @@
         <v>1.0</v>
       </c>
       <c r="C28" t="n">
-        <v>1.1731542348861694</v>
+        <v>0.7297766804695129</v>
       </c>
       <c r="D28" t="n">
         <v>261.5260869750733</v>
       </c>
       <c r="E28" t="n">
-        <v>0.06753670424222946</v>
+        <v>0.042012132704257965</v>
       </c>
       <c r="F28" t="n">
         <v>1.0</v>
@@ -654,13 +604,13 @@
         <v>10.0</v>
       </c>
       <c r="C29" t="n">
-        <v>0.9511350989341736</v>
+        <v>0.591666579246521</v>
       </c>
       <c r="D29" t="n">
         <v>261.6143715155233</v>
       </c>
       <c r="E29" t="n">
-        <v>0.2243632674217224</v>
+        <v>0.1395682394504547</v>
       </c>
       <c r="F29" t="n">
         <v>6.0</v>
@@ -674,13 +624,13 @@
         <v>10.0</v>
       </c>
       <c r="C30" t="n">
-        <v>0.8602044582366943</v>
+        <v>0.5351018905639648</v>
       </c>
       <c r="D30" t="n">
         <v>261.6337953543354</v>
       </c>
       <c r="E30" t="n">
-        <v>0.1465173065662384</v>
+        <v>0.09114309400320053</v>
       </c>
       <c r="F30" t="n">
         <v>6.0</v>
@@ -694,13 +644,13 @@
         <v>10.0</v>
       </c>
       <c r="C31" t="n">
-        <v>0.833429753780365</v>
+        <v>0.5184463858604431</v>
       </c>
       <c r="D31" t="n">
         <v>261.64456146410316</v>
       </c>
       <c r="E31" t="n">
-        <v>0.028472568839788437</v>
+        <v>0.01771175116300583</v>
       </c>
       <c r="F31" t="n">
         <v>6.0</v>
@@ -714,13 +664,13 @@
         <v>10.0</v>
       </c>
       <c r="C32" t="n">
-        <v>0.9158056378364563</v>
+        <v>0.5696893930435181</v>
       </c>
       <c r="D32" t="n">
         <v>261.62780508586667</v>
       </c>
       <c r="E32" t="n">
-        <v>0.13939817249774933</v>
+        <v>0.08671453595161438</v>
       </c>
       <c r="F32" t="n">
         <v>6.0</v>
@@ -734,13 +684,13 @@
         <v>10.0</v>
       </c>
       <c r="C33" t="n">
-        <v>1.073432445526123</v>
+        <v>0.6677433252334595</v>
       </c>
       <c r="D33" t="n">
         <v>261.6266045710891</v>
       </c>
       <c r="E33" t="n">
-        <v>0.288409024477005</v>
+        <v>0.17940877377986908</v>
       </c>
       <c r="F33" t="n">
         <v>6.0</v>
@@ -754,13 +704,13 @@
         <v>1.0</v>
       </c>
       <c r="C34" t="n">
-        <v>1.1081416606903076</v>
+        <v>0.6893346905708313</v>
       </c>
       <c r="D34" t="n">
         <v>261.6963311869112</v>
       </c>
       <c r="E34" t="n">
-        <v>0.23920954763889313</v>
+        <v>0.14880356192588806</v>
       </c>
       <c r="F34" t="n">
         <v>1.0</v>
@@ -774,13 +724,13 @@
         <v>1.0</v>
       </c>
       <c r="C35" t="n">
-        <v>1.0533623695373535</v>
+        <v>0.6552584171295166</v>
       </c>
       <c r="D35" t="n">
         <v>261.7457281617366</v>
       </c>
       <c r="E35" t="n">
-        <v>0.10288845747709274</v>
+        <v>0.06400316953659058</v>
       </c>
       <c r="F35" t="n">
         <v>1.0</v>
@@ -794,13 +744,13 @@
         <v>2.0</v>
       </c>
       <c r="C36" t="n">
-        <v>0.9183313250541687</v>
+        <v>0.5712605714797974</v>
       </c>
       <c r="D36" t="n">
         <v>261.74771242780264</v>
       </c>
       <c r="E36" t="n">
-        <v>0.16437725722789764</v>
+        <v>0.10225311666727066</v>
       </c>
       <c r="F36" t="n">
         <v>1.0</v>
@@ -814,13 +764,13 @@
         <v>1.0</v>
       </c>
       <c r="C37" t="n">
-        <v>0.6471188068389893</v>
+        <v>0.4025490880012512</v>
       </c>
       <c r="D37" t="n">
         <v>261.8530329755303</v>
       </c>
       <c r="E37" t="n">
-        <v>0.28039973974227905</v>
+        <v>0.17442648112773895</v>
       </c>
       <c r="F37" t="n">
         <v>3.0</v>
@@ -834,13 +784,13 @@
         <v>4.0</v>
       </c>
       <c r="C38" t="n">
-        <v>0.5690993070602417</v>
+        <v>0.3540160059928894</v>
       </c>
       <c r="D38" t="n">
         <v>261.8092385280714</v>
       </c>
       <c r="E38" t="n">
-        <v>0.21096783876419067</v>
+        <v>0.13123542070388794</v>
       </c>
       <c r="F38" t="n">
         <v>4.0</v>
@@ -854,13 +804,13 @@
         <v>10.0</v>
       </c>
       <c r="C39" t="n">
-        <v>0.6677214503288269</v>
+        <v>0.4153652489185333</v>
       </c>
       <c r="D39" t="n">
         <v>261.73523225362436</v>
       </c>
       <c r="E39" t="n">
-        <v>0.16649450361728668</v>
+        <v>0.10357017815113068</v>
       </c>
       <c r="F39" t="n">
         <v>6.0</v>
@@ -874,13 +824,13 @@
         <v>1.0</v>
       </c>
       <c r="C40" t="n">
-        <v>0.40551504492759705</v>
+        <v>0.2522561550140381</v>
       </c>
       <c r="D40" t="n">
         <v>261.86063939372787</v>
       </c>
       <c r="E40" t="n">
-        <v>0.26956841349601746</v>
+        <v>0.16768871247768402</v>
       </c>
       <c r="F40" t="n">
         <v>6.0</v>
@@ -894,13 +844,13 @@
         <v>5.0</v>
       </c>
       <c r="C41" t="n">
-        <v>0.26619550585746765</v>
+        <v>0.1655905395746231</v>
       </c>
       <c r="D41" t="n">
         <v>261.9041240218826</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1610601395368576</v>
+        <v>0.10018965601921082</v>
       </c>
       <c r="F41" t="n">
         <v>3.0</v>
@@ -914,13 +864,13 @@
         <v>4.0</v>
       </c>
       <c r="C42" t="n">
-        <v>0.24060335755348206</v>
+        <v>0.14967060089111328</v>
       </c>
       <c r="D42" t="n">
         <v>261.9164291959897</v>
       </c>
       <c r="E42" t="n">
-        <v>0.025917239487171173</v>
+        <v>0.01612217165529728</v>
       </c>
       <c r="F42" t="n">
         <v>3.0</v>
@@ -934,13 +884,13 @@
         <v>4.0</v>
       </c>
       <c r="C43" t="n">
-        <v>0.3815269470214844</v>
+        <v>0.23733405768871307</v>
       </c>
       <c r="D43" t="n">
         <v>261.85269539989224</v>
       </c>
       <c r="E43" t="n">
-        <v>0.2430168092250824</v>
+        <v>0.15117192268371582</v>
       </c>
       <c r="F43" t="n">
         <v>3.0</v>
@@ -954,13 +904,13 @@
         <v>8.0</v>
       </c>
       <c r="C44" t="n">
-        <v>0.4411461353302002</v>
+        <v>0.27442097663879395</v>
       </c>
       <c r="D44" t="n">
         <v>261.84218775469515</v>
       </c>
       <c r="E44" t="n">
-        <v>0.09722606837749481</v>
+        <v>0.06048080697655678</v>
       </c>
       <c r="F44" t="n">
         <v>5.0</v>
@@ -974,13 +924,13 @@
         <v>12.0</v>
       </c>
       <c r="C45" t="n">
-        <v>0.4147675037384033</v>
+        <v>0.2580117881298065</v>
       </c>
       <c r="D45" t="n">
         <v>261.8742012620678</v>
       </c>
       <c r="E45" t="n">
-        <v>0.0824146419763565</v>
+        <v>0.05126715451478958</v>
       </c>
       <c r="F45" t="n">
         <v>6.0</v>
@@ -994,13 +944,13 @@
         <v>1.0</v>
       </c>
       <c r="C46" t="n">
-        <v>0.559756338596344</v>
+        <v>0.3482040762901306</v>
       </c>
       <c r="D46" t="n">
         <v>261.832411431518</v>
       </c>
       <c r="E46" t="n">
-        <v>0.14805088937282562</v>
+        <v>0.09209708124399185</v>
       </c>
       <c r="F46" t="n">
         <v>6.0</v>
@@ -1014,13 +964,13 @@
         <v>6.0</v>
       </c>
       <c r="C47" t="n">
-        <v>0.6999629139900208</v>
+        <v>0.43542152643203735</v>
       </c>
       <c r="D47" t="n">
         <v>261.8009810208278</v>
       </c>
       <c r="E47" t="n">
-        <v>0.1469498574733734</v>
+        <v>0.09141216427087784</v>
       </c>
       <c r="F47" t="n">
         <v>3.0</v>
@@ -1034,13 +984,13 @@
         <v>1.0</v>
       </c>
       <c r="C48" t="n">
-        <v>0.3985292911529541</v>
+        <v>0.24791058897972107</v>
       </c>
       <c r="D48" t="n">
         <v>261.9136333683507</v>
       </c>
       <c r="E48" t="n">
-        <v>0.30655360221862793</v>
+        <v>0.1906958520412445</v>
       </c>
       <c r="F48" t="n">
         <v>3.0</v>
@@ -1054,13 +1004,13 @@
         <v>4.0</v>
       </c>
       <c r="C49" t="n">
-        <v>0.3747617304325104</v>
+        <v>0.23312565684318542</v>
       </c>
       <c r="D49" t="n">
         <v>261.9456724917965</v>
       </c>
       <c r="E49" t="n">
-        <v>0.0677696168422699</v>
+        <v>0.04215701296925545</v>
       </c>
       <c r="F49" t="n">
         <v>3.0</v>
@@ -1074,13 +1024,13 @@
         <v>2.0</v>
       </c>
       <c r="C50" t="n">
-        <v>0.2931596636772156</v>
+        <v>0.18236397206783295</v>
       </c>
       <c r="D50" t="n">
         <v>261.9081444294253</v>
       </c>
       <c r="E50" t="n">
-        <v>0.19104407727718353</v>
+        <v>0.11884157359600067</v>
       </c>
       <c r="F50" t="n">
         <v>4.0</v>
@@ -1094,13 +1044,13 @@
         <v>2.0</v>
       </c>
       <c r="C51" t="n">
-        <v>0.08953952044248581</v>
+        <v>0.05569928139448166</v>
       </c>
       <c r="D51" t="n">
         <v>261.9890906815781</v>
       </c>
       <c r="E51" t="n">
-        <v>0.20371700823307037</v>
+        <v>0.1267249435186386</v>
       </c>
       <c r="F51" t="n">
         <v>1.0</v>
@@ -1114,13 +1064,13 @@
         <v>2.0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.07692065089941025</v>
+        <v>0.047849543392658234</v>
       </c>
       <c r="D52" t="n">
         <v>261.99499261555235</v>
       </c>
       <c r="E52" t="n">
-        <v>0.012963603250682354</v>
+        <v>0.008064186200499535</v>
       </c>
       <c r="F52" t="n">
         <v>1.0</v>
@@ -1134,13 +1084,13 @@
         <v>2.0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.07495752722024918</v>
+        <v>0.046628355979919434</v>
       </c>
       <c r="D53" t="n">
         <v>262.001731797022</v>
       </c>
       <c r="E53" t="n">
-        <v>0.019395161420106888</v>
+        <v>0.012065025046467781</v>
       </c>
       <c r="F53" t="n">
         <v>1.0</v>
@@ -1154,13 +1104,13 @@
         <v>2.0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.07377470284700394</v>
+        <v>0.045892562717199326</v>
       </c>
       <c r="D54" t="n">
         <v>262.0171039955313</v>
       </c>
       <c r="E54" t="n">
-        <v>0.035702068358659744</v>
+        <v>0.022208958864212036</v>
       </c>
       <c r="F54" t="n">
         <v>1.0</v>
@@ -1174,13 +1124,13 @@
         <v>2.0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.059766702353954315</v>
+        <v>0.03717869520187378</v>
       </c>
       <c r="D55" t="n">
         <v>262.0273419598029</v>
       </c>
       <c r="E55" t="n">
-        <v>0.024302326142787933</v>
+        <v>0.015117594040930271</v>
       </c>
       <c r="F55" t="n">
         <v>1.0</v>
@@ -1194,13 +1144,13 @@
         <v>4.0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.12855416536331177</v>
+        <v>0.0799688771367073</v>
       </c>
       <c r="D56" t="n">
         <v>262.02842904452655</v>
       </c>
       <c r="E56" t="n">
-        <v>0.06879103928804398</v>
+        <v>0.04279240220785141</v>
       </c>
       <c r="F56" t="n">
         <v>3.0</v>
@@ -1214,13 +1164,13 @@
         <v>3.0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.10356690734624863</v>
+        <v>0.06442520767450333</v>
       </c>
       <c r="D57" t="n">
         <v>262.03744350084025</v>
       </c>
       <c r="E57" t="n">
-        <v>0.03341617435216904</v>
+        <v>0.020786987617611885</v>
       </c>
       <c r="F57" t="n">
         <v>4.0</v>
@@ -1234,13 +1184,13 @@
         <v>1.0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.0815577432513237</v>
+        <v>0.050734106451272964</v>
       </c>
       <c r="D58" t="n">
         <v>262.03720115376393</v>
       </c>
       <c r="E58" t="n">
-        <v>0.022644149139523506</v>
+        <v>0.01408610213547945</v>
       </c>
       <c r="F58" t="n">
         <v>1.0</v>
@@ -1254,13 +1204,13 @@
         <v>1.0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.02793951891362667</v>
+        <v>0.017380159348249435</v>
       </c>
       <c r="D59" t="n">
         <v>262.0384776220169</v>
       </c>
       <c r="E59" t="n">
-        <v>0.06796745210886002</v>
+        <v>0.042280081659555435</v>
       </c>
       <c r="F59" t="n">
         <v>1.0</v>
@@ -1280,42 +1230,42 @@
         <v>262.025968659323</v>
       </c>
       <c r="E60" t="n">
-        <v>0.02793951891362667</v>
+        <v>0.017380159348249435</v>
       </c>
       <c r="F60" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="s" s="19">
+      <c r="A61" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="B61" s="19" t="n">
+      <c r="B61" s="7" t="n">
         <f>SUM(B19:B60)</f>
         <v>150.0</v>
       </c>
-      <c r="E61" s="19" t="n">
+      <c r="E61" s="7" t="n">
         <f>SUM(E19:E60)</f>
-        <v>6.831668204627931</v>
+        <v>4.249732468277216</v>
       </c>
     </row>
     <row r="62"/>
     <row r="63"/>
     <row r="64"/>
     <row r="65">
-      <c r="A65" t="s" s="19">
+      <c r="A65" t="s" s="7">
         <v>16</v>
       </c>
       <c r="B65" t="n">
         <v>-1.0</v>
       </c>
-      <c r="C65" t="s" s="19">
+      <c r="C65" t="s" s="7">
         <v>17</v>
       </c>
       <c r="D65" t="n">
         <v>-80.046878</v>
       </c>
-      <c r="E65" t="s" s="19">
+      <c r="E65" t="s" s="7">
         <v>18</v>
       </c>
       <c r="F65" t="n">
@@ -1323,37 +1273,37 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s" s="19">
+      <c r="A66" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="B66" t="n" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="C66" t="s" s="19">
+      <c r="B66" t="n" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="C66" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="D66" t="n" s="20">
+      <c r="D66" t="n" s="8">
         <v>-1.0</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="s" s="19">
+      <c r="A67" t="s" s="7">
         <v>21</v>
       </c>
-      <c r="B67" t="n" s="20">
-        <v>3.637298822402954</v>
-      </c>
-      <c r="C67" t="s" s="19">
+      <c r="B67" t="n" s="8">
+        <v>2.2626311779022217</v>
+      </c>
+      <c r="C67" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="D67" t="n" s="20">
-        <v>374.0</v>
-      </c>
-      <c r="E67" t="s" s="19">
+      <c r="D67" t="n" s="8">
+        <v>367.0</v>
+      </c>
+      <c r="E67" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="F67" t="n" s="20">
-        <v>3.637298822402954</v>
+      <c r="F67" t="n" s="8">
+        <v>2.2626311779022217</v>
       </c>
     </row>
     <row r="68"/>
@@ -1405,13 +1355,13 @@
         <v>4.0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.30144205689430237</v>
+        <v>0.18751613795757294</v>
       </c>
       <c r="D71" t="n">
         <v>261.9345977905843</v>
       </c>
       <c r="E71" t="n">
-        <v>0.30144205689430237</v>
+        <v>0.18751613795757294</v>
       </c>
       <c r="F71" t="n">
         <v>2.0</v>
@@ -1425,13 +1375,13 @@
         <v>12.0</v>
       </c>
       <c r="C72" t="n">
-        <v>0.4147675037384033</v>
+        <v>0.2580117881298065</v>
       </c>
       <c r="D72" t="n">
         <v>261.8742012620678</v>
       </c>
       <c r="E72" t="n">
-        <v>0.13037799298763275</v>
+        <v>0.08110341429710388</v>
       </c>
       <c r="F72" t="n">
         <v>6.0</v>
@@ -1445,13 +1395,13 @@
         <v>3.0</v>
       </c>
       <c r="C73" t="n">
-        <v>0.41277188062667847</v>
+        <v>0.25677040219306946</v>
       </c>
       <c r="D73" t="n">
         <v>261.8504227828364</v>
       </c>
       <c r="E73" t="n">
-        <v>0.09090527147054672</v>
+        <v>0.056548867374658585</v>
       </c>
       <c r="F73" t="n">
         <v>2.0</v>
@@ -1465,13 +1415,13 @@
         <v>8.0</v>
       </c>
       <c r="C74" t="n">
-        <v>0.4411461353302002</v>
+        <v>0.27442097663879395</v>
       </c>
       <c r="D74" t="n">
         <v>261.84218775469515</v>
       </c>
       <c r="E74" t="n">
-        <v>0.03253420442342758</v>
+        <v>0.020238345488905907</v>
       </c>
       <c r="F74" t="n">
         <v>5.0</v>
@@ -1485,13 +1435,13 @@
         <v>3.0</v>
       </c>
       <c r="C75" t="n">
-        <v>0.5833421349525452</v>
+        <v>0.36287596821784973</v>
       </c>
       <c r="D75" t="n">
         <v>261.84567371889716</v>
       </c>
       <c r="E75" t="n">
-        <v>0.22648894786834717</v>
+        <v>0.14089053869247437</v>
       </c>
       <c r="F75" t="n">
         <v>2.0</v>
@@ -1505,13 +1455,13 @@
         <v>1.0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.559756338596344</v>
+        <v>0.3482040762901306</v>
       </c>
       <c r="D76" t="n">
         <v>261.832411431518</v>
       </c>
       <c r="E76" t="n">
-        <v>0.06408242136240005</v>
+        <v>0.03986334800720215</v>
       </c>
       <c r="F76" t="n">
         <v>6.0</v>
@@ -1525,13 +1475,13 @@
         <v>3.0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.5436442494392395</v>
+        <v>0.3381813168525696</v>
       </c>
       <c r="D77" t="n">
         <v>261.80355109326473</v>
       </c>
       <c r="E77" t="n">
-        <v>0.11930186301469803</v>
+        <v>0.07421335577964783</v>
       </c>
       <c r="F77" t="n">
         <v>2.0</v>
@@ -1545,13 +1495,13 @@
         <v>1.0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.49632975459098816</v>
+        <v>0.30874869227409363</v>
       </c>
       <c r="D78" t="n">
         <v>261.80366879016594</v>
       </c>
       <c r="E78" t="n">
-        <v>0.10480140894651413</v>
+        <v>0.06519314646720886</v>
       </c>
       <c r="F78" t="n">
         <v>2.0</v>
@@ -1565,13 +1515,13 @@
         <v>4.0</v>
       </c>
       <c r="C79" t="n">
-        <v>0.5023859739303589</v>
+        <v>0.3125160336494446</v>
       </c>
       <c r="D79" t="n">
         <v>261.7925079122199</v>
       </c>
       <c r="E79" t="n">
-        <v>0.05615795776247978</v>
+        <v>0.034933824092149734</v>
       </c>
       <c r="F79" t="n">
         <v>2.0</v>
@@ -1585,13 +1535,13 @@
         <v>4.0</v>
       </c>
       <c r="C80" t="n">
-        <v>0.39102786779403687</v>
+        <v>0.2432442307472229</v>
       </c>
       <c r="D80" t="n">
         <v>261.8399552608657</v>
       </c>
       <c r="E80" t="n">
-        <v>0.21286500990390778</v>
+        <v>0.13241559267044067</v>
       </c>
       <c r="F80" t="n">
         <v>2.0</v>
@@ -1605,13 +1555,13 @@
         <v>1.0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.48756301403045654</v>
+        <v>0.30329522490501404</v>
       </c>
       <c r="D81" t="n">
         <v>261.79625441958456</v>
       </c>
       <c r="E81" t="n">
-        <v>0.09934674948453903</v>
+        <v>0.06180000305175781</v>
       </c>
       <c r="F81" t="n">
         <v>3.0</v>
@@ -1625,13 +1575,13 @@
         <v>10.0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.6677214503288269</v>
+        <v>0.4153652489185333</v>
       </c>
       <c r="D82" t="n">
         <v>261.73523225362436</v>
       </c>
       <c r="E82" t="n">
-        <v>0.22453835606575012</v>
+        <v>0.13967715203762054</v>
       </c>
       <c r="F82" t="n">
         <v>6.0</v>
@@ -1645,13 +1595,13 @@
         <v>10.0</v>
       </c>
       <c r="C83" t="n">
-        <v>1.073432445526123</v>
+        <v>0.6677433252334595</v>
       </c>
       <c r="D83" t="n">
         <v>261.6266045710891</v>
       </c>
       <c r="E83" t="n">
-        <v>0.4563227593898773</v>
+        <v>0.28386181592941284</v>
       </c>
       <c r="F83" t="n">
         <v>6.0</v>
@@ -1665,13 +1615,13 @@
         <v>5.0</v>
       </c>
       <c r="C84" t="n">
-        <v>1.1121973991394043</v>
+        <v>0.6918575763702393</v>
       </c>
       <c r="D84" t="n">
         <v>261.55286056275264</v>
       </c>
       <c r="E84" t="n">
-        <v>0.22226640582084656</v>
+        <v>0.13826385140419006</v>
       </c>
       <c r="F84" t="n">
         <v>3.0</v>
@@ -1685,13 +1635,13 @@
         <v>8.0</v>
       </c>
       <c r="C85" t="n">
-        <v>0.9836602210998535</v>
+        <v>0.6118992567062378</v>
       </c>
       <c r="D85" t="n">
         <v>261.6216537846275</v>
       </c>
       <c r="E85" t="n">
-        <v>0.1432289034128189</v>
+        <v>0.08909749239683151</v>
       </c>
       <c r="F85" t="n">
         <v>3.0</v>
@@ -1705,13 +1655,13 @@
         <v>10.0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.9511350989341736</v>
+        <v>0.591666579246521</v>
       </c>
       <c r="D86" t="n">
         <v>261.6143715155233</v>
       </c>
       <c r="E86" t="n">
-        <v>0.09676468372344971</v>
+        <v>0.06019379198551178</v>
       </c>
       <c r="F86" t="n">
         <v>6.0</v>
@@ -1725,13 +1675,13 @@
         <v>10.0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.9158056378364563</v>
+        <v>0.5696893930435181</v>
       </c>
       <c r="D87" t="n">
         <v>261.62780508586667</v>
       </c>
       <c r="E87" t="n">
-        <v>0.03647772595286369</v>
+        <v>0.02269146777689457</v>
       </c>
       <c r="F87" t="n">
         <v>6.0</v>
@@ -1745,13 +1695,13 @@
         <v>10.0</v>
       </c>
       <c r="C88" t="n">
-        <v>0.8602044582366943</v>
+        <v>0.5351018905639648</v>
       </c>
       <c r="D88" t="n">
         <v>261.6337953543354</v>
       </c>
       <c r="E88" t="n">
-        <v>0.11803000420331955</v>
+        <v>0.07342217862606049</v>
       </c>
       <c r="F88" t="n">
         <v>6.0</v>
@@ -1765,13 +1715,13 @@
         <v>10.0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.833429753780365</v>
+        <v>0.5184463858604431</v>
       </c>
       <c r="D89" t="n">
         <v>261.64456146410316</v>
       </c>
       <c r="E89" t="n">
-        <v>0.028472568839788437</v>
+        <v>0.01771175116300583</v>
       </c>
       <c r="F89" t="n">
         <v>6.0</v>
@@ -1785,13 +1735,13 @@
         <v>1.0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.40551504492759705</v>
+        <v>0.2522561550140381</v>
       </c>
       <c r="D90" t="n">
         <v>261.86063939372787</v>
       </c>
       <c r="E90" t="n">
-        <v>0.45106178522109985</v>
+        <v>0.28058916330337524</v>
       </c>
       <c r="F90" t="n">
         <v>6.0</v>
@@ -1805,13 +1755,13 @@
         <v>6.0</v>
       </c>
       <c r="C91" t="n">
-        <v>0.340213805437088</v>
+        <v>0.21163465082645416</v>
       </c>
       <c r="D91" t="n">
         <v>261.89989924983104</v>
       </c>
       <c r="E91" t="n">
-        <v>0.08161762356758118</v>
+        <v>0.050771359354257584</v>
       </c>
       <c r="F91" t="n">
         <v>2.0</v>
@@ -1831,42 +1781,42 @@
         <v>262.025968659323</v>
       </c>
       <c r="E92" t="n">
-        <v>0.340213805437088</v>
+        <v>0.21163465082645416</v>
       </c>
       <c r="F92" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="s" s="19">
+      <c r="A93" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="B93" s="19" t="n">
+      <c r="B93" s="7" t="n">
         <f>SUM(B70:B92)</f>
         <v>124.0</v>
       </c>
-      <c r="E93" s="19" t="n">
+      <c r="E93" s="7" t="n">
         <f>SUM(E70:E92)</f>
-        <v>3.6372985057532787</v>
+        <v>2.2626312486827374</v>
       </c>
     </row>
     <row r="94"/>
     <row r="95"/>
     <row r="96"/>
     <row r="97">
-      <c r="A97" t="s" s="19">
+      <c r="A97" t="s" s="7">
         <v>16</v>
       </c>
       <c r="B97" t="n">
         <v>-1.0</v>
       </c>
-      <c r="C97" t="s" s="19">
+      <c r="C97" t="s" s="7">
         <v>17</v>
       </c>
       <c r="D97" t="n">
         <v>-80.046878</v>
       </c>
-      <c r="E97" t="s" s="19">
+      <c r="E97" t="s" s="7">
         <v>18</v>
       </c>
       <c r="F97" t="n">
@@ -1874,37 +1824,37 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="s" s="19">
+      <c r="A98" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="B98" t="n" s="19">
+      <c r="B98" t="n" s="7">
         <v>2.0</v>
       </c>
-      <c r="C98" t="s" s="19">
+      <c r="C98" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="D98" t="n" s="20">
+      <c r="D98" t="n" s="8">
         <v>-1.0</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="s" s="19">
+      <c r="A99" t="s" s="7">
         <v>21</v>
       </c>
-      <c r="B99" t="n" s="20">
-        <v>3.9416000843048096</v>
-      </c>
-      <c r="C99" t="s" s="19">
+      <c r="B99" t="n" s="8">
+        <v>2.4519267082214355</v>
+      </c>
+      <c r="C99" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="D99" t="n" s="20">
-        <v>377.0</v>
-      </c>
-      <c r="E99" t="s" s="19">
+      <c r="D99" t="n" s="8">
+        <v>370.0</v>
+      </c>
+      <c r="E99" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="F99" t="n" s="20">
-        <v>3.9416000843048096</v>
+      <c r="F99" t="n" s="8">
+        <v>2.4519267082214355</v>
       </c>
     </row>
     <row r="100"/>
@@ -1950,19 +1900,19 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>34.0</v>
+        <v>40.0</v>
       </c>
       <c r="B103" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C103" t="n">
-        <v>0.4929746091365814</v>
+        <v>0.06442520767450333</v>
       </c>
       <c r="D103" t="n">
-        <v>261.8645538790942</v>
+        <v>262.03744350084025</v>
       </c>
       <c r="E103" t="n">
-        <v>0.4929746091365814</v>
+        <v>0.06442520767450333</v>
       </c>
       <c r="F103" t="n">
         <v>4.0</v>
@@ -1970,19 +1920,19 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>33.0</v>
+        <v>39.0</v>
       </c>
       <c r="B104" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="C104" t="n">
-        <v>0.6471188068389893</v>
+        <v>0.0799688771367073</v>
       </c>
       <c r="D104" t="n">
-        <v>261.8530329755303</v>
+        <v>262.02842904452655</v>
       </c>
       <c r="E104" t="n">
-        <v>0.1785203516483307</v>
+        <v>0.020786987617611885</v>
       </c>
       <c r="F104" t="n">
         <v>3.0</v>
@@ -1990,79 +1940,79 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>18.0</v>
+        <v>47.0</v>
       </c>
       <c r="B105" t="n">
-        <v>10.0</v>
+        <v>4.0</v>
       </c>
       <c r="C105" t="n">
-        <v>1.073432445526123</v>
+        <v>0.23312565684318542</v>
       </c>
       <c r="D105" t="n">
-        <v>261.6266045710891</v>
+        <v>261.9456724917965</v>
       </c>
       <c r="E105" t="n">
-        <v>0.49173110723495483</v>
+        <v>0.1674681156873703</v>
       </c>
       <c r="F105" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>26.0</v>
+        <v>48.0</v>
       </c>
       <c r="B106" t="n">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="C106" t="n">
-        <v>0.9511350989341736</v>
+        <v>0.24791058897972107</v>
       </c>
       <c r="D106" t="n">
-        <v>261.6143715155233</v>
+        <v>261.9136333683507</v>
       </c>
       <c r="E106" t="n">
-        <v>0.26614075899124146</v>
+        <v>0.04215701296925545</v>
       </c>
       <c r="F106" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>27.0</v>
+        <v>59.0</v>
       </c>
       <c r="B107" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="C107" t="n">
-        <v>0.9158056378364563</v>
+        <v>0.43542152643203735</v>
       </c>
       <c r="D107" t="n">
-        <v>261.62780508586667</v>
+        <v>261.8009810208278</v>
       </c>
       <c r="E107" t="n">
-        <v>0.03647772595286369</v>
+        <v>0.1906958520412445</v>
       </c>
       <c r="F107" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>29.0</v>
+        <v>57.0</v>
       </c>
       <c r="B108" t="n">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="C108" t="n">
-        <v>0.8602044582366943</v>
+        <v>0.3482040762901306</v>
       </c>
       <c r="D108" t="n">
-        <v>261.6337953543354</v>
+        <v>261.832411431518</v>
       </c>
       <c r="E108" t="n">
-        <v>0.11803000420331955</v>
+        <v>0.09141216427087784</v>
       </c>
       <c r="F108" t="n">
         <v>6.0</v>
@@ -2070,19 +2020,19 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>28.0</v>
+        <v>49.0</v>
       </c>
       <c r="B109" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="C109" t="n">
-        <v>0.833429753780365</v>
+        <v>0.2580117881298065</v>
       </c>
       <c r="D109" t="n">
-        <v>261.64456146410316</v>
+        <v>261.8742012620678</v>
       </c>
       <c r="E109" t="n">
-        <v>0.028472568839788437</v>
+        <v>0.09209708124399185</v>
       </c>
       <c r="F109" t="n">
         <v>6.0</v>
@@ -2090,79 +2040,79 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>30.0</v>
+        <v>50.0</v>
       </c>
       <c r="B110" t="n">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="C110" t="n">
-        <v>0.6677214503288269</v>
+        <v>0.27442097663879395</v>
       </c>
       <c r="D110" t="n">
-        <v>261.73523225362436</v>
+        <v>261.84218775469515</v>
       </c>
       <c r="E110" t="n">
-        <v>0.19035542011260986</v>
+        <v>0.05126715451478958</v>
       </c>
       <c r="F110" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>31.0</v>
+        <v>45.0</v>
       </c>
       <c r="B111" t="n">
         <v>4.0</v>
       </c>
       <c r="C111" t="n">
-        <v>0.5690993070602417</v>
+        <v>0.23733405768871307</v>
       </c>
       <c r="D111" t="n">
-        <v>261.8092385280714</v>
+        <v>261.85269539989224</v>
       </c>
       <c r="E111" t="n">
-        <v>0.16649450361728668</v>
+        <v>0.06048080697655678</v>
       </c>
       <c r="F111" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>36.0</v>
+        <v>44.0</v>
       </c>
       <c r="B112" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C112" t="n">
-        <v>0.40551504492759705</v>
+        <v>0.18236397206783295</v>
       </c>
       <c r="D112" t="n">
-        <v>261.86063939372787</v>
+        <v>261.9081444294253</v>
       </c>
       <c r="E112" t="n">
-        <v>0.17018213868141174</v>
+        <v>0.07496415823698044</v>
       </c>
       <c r="F112" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>42.0</v>
+        <v>41.0</v>
       </c>
       <c r="B113" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C113" t="n">
-        <v>0.26619550585746765</v>
+        <v>0.14967060089111328</v>
       </c>
       <c r="D113" t="n">
-        <v>261.9041240218826</v>
+        <v>261.9164291959897</v>
       </c>
       <c r="E113" t="n">
-        <v>0.1610601395368576</v>
+        <v>0.14903001487255096</v>
       </c>
       <c r="F113" t="n">
         <v>3.0</v>
@@ -2170,19 +2120,19 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>41.0</v>
+        <v>42.0</v>
       </c>
       <c r="B114" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C114" t="n">
-        <v>0.24060335755348206</v>
+        <v>0.1655905395746231</v>
       </c>
       <c r="D114" t="n">
-        <v>261.9164291959897</v>
+        <v>261.9041240218826</v>
       </c>
       <c r="E114" t="n">
-        <v>0.025917239487171173</v>
+        <v>0.01612217165529728</v>
       </c>
       <c r="F114" t="n">
         <v>3.0</v>
@@ -2190,79 +2140,79 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>44.0</v>
+        <v>36.0</v>
       </c>
       <c r="B115" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C115" t="n">
-        <v>0.2931596636772156</v>
+        <v>0.2522561550140381</v>
       </c>
       <c r="D115" t="n">
-        <v>261.9081444294253</v>
+        <v>261.86063939372787</v>
       </c>
       <c r="E115" t="n">
-        <v>0.23957358300685883</v>
+        <v>0.10018965601921082</v>
       </c>
       <c r="F115" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>45.0</v>
+        <v>31.0</v>
       </c>
       <c r="B116" t="n">
         <v>4.0</v>
       </c>
       <c r="C116" t="n">
-        <v>0.3815269470214844</v>
+        <v>0.3540160059928894</v>
       </c>
       <c r="D116" t="n">
-        <v>261.85269539989224</v>
+        <v>261.8092385280714</v>
       </c>
       <c r="E116" t="n">
-        <v>0.1205088198184967</v>
+        <v>0.10586412250995636</v>
       </c>
       <c r="F116" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>50.0</v>
+        <v>30.0</v>
       </c>
       <c r="B117" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="C117" t="n">
-        <v>0.4411461353302002</v>
+        <v>0.4153652489185333</v>
       </c>
       <c r="D117" t="n">
-        <v>261.84218775469515</v>
+        <v>261.73523225362436</v>
       </c>
       <c r="E117" t="n">
-        <v>0.09722606837749481</v>
+        <v>0.10357017815113068</v>
       </c>
       <c r="F117" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>49.0</v>
+        <v>28.0</v>
       </c>
       <c r="B118" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="C118" t="n">
-        <v>0.4147675037384033</v>
+        <v>0.5184463858604431</v>
       </c>
       <c r="D118" t="n">
-        <v>261.8742012620678</v>
+        <v>261.64456146410316</v>
       </c>
       <c r="E118" t="n">
-        <v>0.0824146419763565</v>
+        <v>0.11841318756341934</v>
       </c>
       <c r="F118" t="n">
         <v>6.0</v>
@@ -2270,19 +2220,19 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>57.0</v>
+        <v>29.0</v>
       </c>
       <c r="B119" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="C119" t="n">
-        <v>0.559756338596344</v>
+        <v>0.5351018905639648</v>
       </c>
       <c r="D119" t="n">
-        <v>261.832411431518</v>
+        <v>261.6337953543354</v>
       </c>
       <c r="E119" t="n">
-        <v>0.14805088937282562</v>
+        <v>0.01771175116300583</v>
       </c>
       <c r="F119" t="n">
         <v>6.0</v>
@@ -2290,79 +2240,79 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>59.0</v>
+        <v>27.0</v>
       </c>
       <c r="B120" t="n">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="C120" t="n">
-        <v>0.6999629139900208</v>
+        <v>0.5696893930435181</v>
       </c>
       <c r="D120" t="n">
-        <v>261.8009810208278</v>
+        <v>261.62780508586667</v>
       </c>
       <c r="E120" t="n">
-        <v>0.1469498574733734</v>
+        <v>0.07342217862606049</v>
       </c>
       <c r="F120" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>48.0</v>
+        <v>26.0</v>
       </c>
       <c r="B121" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="C121" t="n">
-        <v>0.3985292911529541</v>
+        <v>0.591666579246521</v>
       </c>
       <c r="D121" t="n">
-        <v>261.9136333683507</v>
+        <v>261.6143715155233</v>
       </c>
       <c r="E121" t="n">
-        <v>0.30655360221862793</v>
+        <v>0.02269146777689457</v>
       </c>
       <c r="F121" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>47.0</v>
+        <v>18.0</v>
       </c>
       <c r="B122" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
       <c r="C122" t="n">
-        <v>0.3747617304325104</v>
+        <v>0.6677433252334595</v>
       </c>
       <c r="D122" t="n">
-        <v>261.9456724917965</v>
+        <v>261.6266045710891</v>
       </c>
       <c r="E122" t="n">
-        <v>0.0677696168422699</v>
+        <v>0.16555650532245636</v>
       </c>
       <c r="F122" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>39.0</v>
+        <v>33.0</v>
       </c>
       <c r="B123" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="C123" t="n">
-        <v>0.12855416536331177</v>
+        <v>0.4025490880012512</v>
       </c>
       <c r="D123" t="n">
-        <v>262.02842904452655</v>
+        <v>261.8530329755303</v>
       </c>
       <c r="E123" t="n">
-        <v>0.26921379566192627</v>
+        <v>0.3058880567550659</v>
       </c>
       <c r="F123" t="n">
         <v>3.0</v>
@@ -2370,19 +2320,19 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>40.0</v>
+        <v>34.0</v>
       </c>
       <c r="B124" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C124" t="n">
-        <v>0.10356690734624863</v>
+        <v>0.30666160583496094</v>
       </c>
       <c r="D124" t="n">
-        <v>262.03744350084025</v>
+        <v>261.8645538790942</v>
       </c>
       <c r="E124" t="n">
-        <v>0.03341617435216904</v>
+        <v>0.11105102300643921</v>
       </c>
       <c r="F124" t="n">
         <v>4.0</v>
@@ -2402,42 +2352,42 @@
         <v>262.025968659323</v>
       </c>
       <c r="E125" t="n">
-        <v>0.10356690734624863</v>
+        <v>0.30666160583496094</v>
       </c>
       <c r="F125" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="s" s="19">
+      <c r="A126" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="B126" s="19" t="n">
+      <c r="B126" s="7" t="n">
         <f>SUM(B102:B125)</f>
         <v>121.0</v>
       </c>
-      <c r="E126" s="19" t="n">
+      <c r="E126" s="7" t="n">
         <f>SUM(E102:E125)</f>
-        <v>3.941600523889065</v>
+        <v>2.4519264604896307</v>
       </c>
     </row>
     <row r="127"/>
     <row r="128"/>
     <row r="129"/>
     <row r="130">
-      <c r="A130" t="s" s="19">
+      <c r="A130" t="s" s="7">
         <v>16</v>
       </c>
       <c r="B130" t="n">
         <v>-1.0</v>
       </c>
-      <c r="C130" t="s" s="19">
+      <c r="C130" t="s" s="7">
         <v>17</v>
       </c>
       <c r="D130" t="n">
         <v>-80.046878</v>
       </c>
-      <c r="E130" t="s" s="19">
+      <c r="E130" t="s" s="7">
         <v>18</v>
       </c>
       <c r="F130" t="n">
@@ -2445,37 +2395,37 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="s" s="19">
+      <c r="A131" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="B131" t="n" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="C131" t="s" s="19">
+      <c r="B131" t="n" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="C131" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="D131" t="n" s="20">
+      <c r="D131" t="n" s="8">
         <v>-1.0</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="s" s="19">
+      <c r="A132" t="s" s="7">
         <v>21</v>
       </c>
-      <c r="B132" t="n" s="20">
-        <v>3.637298822402954</v>
-      </c>
-      <c r="C132" t="s" s="19">
+      <c r="B132" t="n" s="8">
+        <v>2.2626311779022217</v>
+      </c>
+      <c r="C132" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="D132" t="n" s="20">
-        <v>374.0</v>
-      </c>
-      <c r="E132" t="s" s="19">
+      <c r="D132" t="n" s="8">
+        <v>367.0</v>
+      </c>
+      <c r="E132" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="F132" t="n" s="20">
-        <v>3.637298822402954</v>
+      <c r="F132" t="n" s="8">
+        <v>2.2626311779022217</v>
       </c>
     </row>
     <row r="133"/>
@@ -2527,13 +2477,13 @@
         <v>4.0</v>
       </c>
       <c r="C136" t="n">
-        <v>0.30144205689430237</v>
+        <v>0.18751613795757294</v>
       </c>
       <c r="D136" t="n">
         <v>261.9345977905843</v>
       </c>
       <c r="E136" t="n">
-        <v>0.30144205689430237</v>
+        <v>0.18751613795757294</v>
       </c>
       <c r="F136" t="n">
         <v>2.0</v>
@@ -2547,13 +2497,13 @@
         <v>12.0</v>
       </c>
       <c r="C137" t="n">
-        <v>0.4147675037384033</v>
+        <v>0.2580117881298065</v>
       </c>
       <c r="D137" t="n">
         <v>261.8742012620678</v>
       </c>
       <c r="E137" t="n">
-        <v>0.13037799298763275</v>
+        <v>0.08110341429710388</v>
       </c>
       <c r="F137" t="n">
         <v>6.0</v>
@@ -2567,13 +2517,13 @@
         <v>3.0</v>
       </c>
       <c r="C138" t="n">
-        <v>0.41277188062667847</v>
+        <v>0.25677040219306946</v>
       </c>
       <c r="D138" t="n">
         <v>261.8504227828364</v>
       </c>
       <c r="E138" t="n">
-        <v>0.09090527147054672</v>
+        <v>0.056548867374658585</v>
       </c>
       <c r="F138" t="n">
         <v>2.0</v>
@@ -2587,13 +2537,13 @@
         <v>8.0</v>
       </c>
       <c r="C139" t="n">
-        <v>0.4411461353302002</v>
+        <v>0.27442097663879395</v>
       </c>
       <c r="D139" t="n">
         <v>261.84218775469515</v>
       </c>
       <c r="E139" t="n">
-        <v>0.03253420442342758</v>
+        <v>0.020238345488905907</v>
       </c>
       <c r="F139" t="n">
         <v>5.0</v>
@@ -2607,13 +2557,13 @@
         <v>3.0</v>
       </c>
       <c r="C140" t="n">
-        <v>0.5833421349525452</v>
+        <v>0.36287596821784973</v>
       </c>
       <c r="D140" t="n">
         <v>261.84567371889716</v>
       </c>
       <c r="E140" t="n">
-        <v>0.22648894786834717</v>
+        <v>0.14089053869247437</v>
       </c>
       <c r="F140" t="n">
         <v>2.0</v>
@@ -2627,13 +2577,13 @@
         <v>1.0</v>
       </c>
       <c r="C141" t="n">
-        <v>0.559756338596344</v>
+        <v>0.3482040762901306</v>
       </c>
       <c r="D141" t="n">
         <v>261.832411431518</v>
       </c>
       <c r="E141" t="n">
-        <v>0.06408242136240005</v>
+        <v>0.03986334800720215</v>
       </c>
       <c r="F141" t="n">
         <v>6.0</v>
@@ -2647,13 +2597,13 @@
         <v>3.0</v>
       </c>
       <c r="C142" t="n">
-        <v>0.5436442494392395</v>
+        <v>0.3381813168525696</v>
       </c>
       <c r="D142" t="n">
         <v>261.80355109326473</v>
       </c>
       <c r="E142" t="n">
-        <v>0.11930186301469803</v>
+        <v>0.07421335577964783</v>
       </c>
       <c r="F142" t="n">
         <v>2.0</v>
@@ -2667,13 +2617,13 @@
         <v>1.0</v>
       </c>
       <c r="C143" t="n">
-        <v>0.49632975459098816</v>
+        <v>0.30874869227409363</v>
       </c>
       <c r="D143" t="n">
         <v>261.80366879016594</v>
       </c>
       <c r="E143" t="n">
-        <v>0.10480140894651413</v>
+        <v>0.06519314646720886</v>
       </c>
       <c r="F143" t="n">
         <v>2.0</v>
@@ -2687,13 +2637,13 @@
         <v>4.0</v>
       </c>
       <c r="C144" t="n">
-        <v>0.5023859739303589</v>
+        <v>0.3125160336494446</v>
       </c>
       <c r="D144" t="n">
         <v>261.7925079122199</v>
       </c>
       <c r="E144" t="n">
-        <v>0.05615795776247978</v>
+        <v>0.034933824092149734</v>
       </c>
       <c r="F144" t="n">
         <v>2.0</v>
@@ -2707,13 +2657,13 @@
         <v>4.0</v>
       </c>
       <c r="C145" t="n">
-        <v>0.39102786779403687</v>
+        <v>0.2432442307472229</v>
       </c>
       <c r="D145" t="n">
         <v>261.8399552608657</v>
       </c>
       <c r="E145" t="n">
-        <v>0.21286500990390778</v>
+        <v>0.13241559267044067</v>
       </c>
       <c r="F145" t="n">
         <v>2.0</v>
@@ -2727,13 +2677,13 @@
         <v>1.0</v>
       </c>
       <c r="C146" t="n">
-        <v>0.48756301403045654</v>
+        <v>0.30329522490501404</v>
       </c>
       <c r="D146" t="n">
         <v>261.79625441958456</v>
       </c>
       <c r="E146" t="n">
-        <v>0.09934674948453903</v>
+        <v>0.06180000305175781</v>
       </c>
       <c r="F146" t="n">
         <v>3.0</v>
@@ -2747,13 +2697,13 @@
         <v>10.0</v>
       </c>
       <c r="C147" t="n">
-        <v>0.6677214503288269</v>
+        <v>0.4153652489185333</v>
       </c>
       <c r="D147" t="n">
         <v>261.73523225362436</v>
       </c>
       <c r="E147" t="n">
-        <v>0.22453835606575012</v>
+        <v>0.13967715203762054</v>
       </c>
       <c r="F147" t="n">
         <v>6.0</v>
@@ -2767,13 +2717,13 @@
         <v>10.0</v>
       </c>
       <c r="C148" t="n">
-        <v>1.073432445526123</v>
+        <v>0.6677433252334595</v>
       </c>
       <c r="D148" t="n">
         <v>261.6266045710891</v>
       </c>
       <c r="E148" t="n">
-        <v>0.4563227593898773</v>
+        <v>0.28386181592941284</v>
       </c>
       <c r="F148" t="n">
         <v>6.0</v>
@@ -2787,13 +2737,13 @@
         <v>5.0</v>
       </c>
       <c r="C149" t="n">
-        <v>1.1121973991394043</v>
+        <v>0.6918575763702393</v>
       </c>
       <c r="D149" t="n">
         <v>261.55286056275264</v>
       </c>
       <c r="E149" t="n">
-        <v>0.22226640582084656</v>
+        <v>0.13826385140419006</v>
       </c>
       <c r="F149" t="n">
         <v>3.0</v>
@@ -2807,13 +2757,13 @@
         <v>8.0</v>
       </c>
       <c r="C150" t="n">
-        <v>0.9836602210998535</v>
+        <v>0.6118992567062378</v>
       </c>
       <c r="D150" t="n">
         <v>261.6216537846275</v>
       </c>
       <c r="E150" t="n">
-        <v>0.1432289034128189</v>
+        <v>0.08909749239683151</v>
       </c>
       <c r="F150" t="n">
         <v>3.0</v>
@@ -2827,13 +2777,13 @@
         <v>10.0</v>
       </c>
       <c r="C151" t="n">
-        <v>0.9511350989341736</v>
+        <v>0.591666579246521</v>
       </c>
       <c r="D151" t="n">
         <v>261.6143715155233</v>
       </c>
       <c r="E151" t="n">
-        <v>0.09676468372344971</v>
+        <v>0.06019379198551178</v>
       </c>
       <c r="F151" t="n">
         <v>6.0</v>
@@ -2847,13 +2797,13 @@
         <v>10.0</v>
       </c>
       <c r="C152" t="n">
-        <v>0.9158056378364563</v>
+        <v>0.5696893930435181</v>
       </c>
       <c r="D152" t="n">
         <v>261.62780508586667</v>
       </c>
       <c r="E152" t="n">
-        <v>0.03647772595286369</v>
+        <v>0.02269146777689457</v>
       </c>
       <c r="F152" t="n">
         <v>6.0</v>
@@ -2867,13 +2817,13 @@
         <v>10.0</v>
       </c>
       <c r="C153" t="n">
-        <v>0.8602044582366943</v>
+        <v>0.5351018905639648</v>
       </c>
       <c r="D153" t="n">
         <v>261.6337953543354</v>
       </c>
       <c r="E153" t="n">
-        <v>0.11803000420331955</v>
+        <v>0.07342217862606049</v>
       </c>
       <c r="F153" t="n">
         <v>6.0</v>
@@ -2887,13 +2837,13 @@
         <v>10.0</v>
       </c>
       <c r="C154" t="n">
-        <v>0.833429753780365</v>
+        <v>0.5184463858604431</v>
       </c>
       <c r="D154" t="n">
         <v>261.64456146410316</v>
       </c>
       <c r="E154" t="n">
-        <v>0.028472568839788437</v>
+        <v>0.01771175116300583</v>
       </c>
       <c r="F154" t="n">
         <v>6.0</v>
@@ -2907,13 +2857,13 @@
         <v>1.0</v>
       </c>
       <c r="C155" t="n">
-        <v>0.40551504492759705</v>
+        <v>0.2522561550140381</v>
       </c>
       <c r="D155" t="n">
         <v>261.86063939372787</v>
       </c>
       <c r="E155" t="n">
-        <v>0.45106178522109985</v>
+        <v>0.28058916330337524</v>
       </c>
       <c r="F155" t="n">
         <v>6.0</v>
@@ -2927,13 +2877,13 @@
         <v>6.0</v>
       </c>
       <c r="C156" t="n">
-        <v>0.340213805437088</v>
+        <v>0.21163465082645416</v>
       </c>
       <c r="D156" t="n">
         <v>261.89989924983104</v>
       </c>
       <c r="E156" t="n">
-        <v>0.08161762356758118</v>
+        <v>0.050771359354257584</v>
       </c>
       <c r="F156" t="n">
         <v>2.0</v>
@@ -2953,42 +2903,42 @@
         <v>262.025968659323</v>
       </c>
       <c r="E157" t="n">
-        <v>0.340213805437088</v>
+        <v>0.21163465082645416</v>
       </c>
       <c r="F157" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="s" s="19">
+      <c r="A158" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="B158" s="19" t="n">
+      <c r="B158" s="7" t="n">
         <f>SUM(B135:B157)</f>
         <v>124.0</v>
       </c>
-      <c r="E158" s="19" t="n">
+      <c r="E158" s="7" t="n">
         <f>SUM(E135:E157)</f>
-        <v>3.6372985057532787</v>
+        <v>2.2626312486827374</v>
       </c>
     </row>
     <row r="159"/>
     <row r="160"/>
     <row r="161"/>
     <row r="162">
-      <c r="A162" t="s" s="19">
+      <c r="A162" t="s" s="7">
         <v>16</v>
       </c>
       <c r="B162" t="n">
         <v>-1.0</v>
       </c>
-      <c r="C162" t="s" s="19">
+      <c r="C162" t="s" s="7">
         <v>17</v>
       </c>
       <c r="D162" t="n">
         <v>-80.046878</v>
       </c>
-      <c r="E162" t="s" s="19">
+      <c r="E162" t="s" s="7">
         <v>18</v>
       </c>
       <c r="F162" t="n">
@@ -2996,37 +2946,37 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="s" s="19">
+      <c r="A163" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="B163" t="n" s="19">
+      <c r="B163" t="n" s="7">
         <v>4.0</v>
       </c>
-      <c r="C163" t="s" s="19">
+      <c r="C163" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="D163" t="n" s="20">
+      <c r="D163" t="n" s="8">
         <v>-1.0</v>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="s" s="19">
+      <c r="A164" t="s" s="7">
         <v>21</v>
       </c>
-      <c r="B164" t="n" s="20">
-        <v>3.7400689125061035</v>
-      </c>
-      <c r="C164" t="s" s="19">
+      <c r="B164" t="n" s="8">
+        <v>2.3265609741210938</v>
+      </c>
+      <c r="C164" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="D164" t="n" s="20">
-        <v>362.0</v>
-      </c>
-      <c r="E164" t="s" s="19">
+      <c r="D164" t="n" s="8">
+        <v>355.0</v>
+      </c>
+      <c r="E164" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="F164" t="n" s="20">
-        <v>3.7400689125061035</v>
+      <c r="F164" t="n" s="8">
+        <v>2.3265609741210938</v>
       </c>
     </row>
     <row r="165"/>
@@ -3078,13 +3028,13 @@
         <v>3.0</v>
       </c>
       <c r="C168" t="n">
-        <v>0.10356690734624863</v>
+        <v>0.06442520767450333</v>
       </c>
       <c r="D168" t="n">
         <v>262.03744350084025</v>
       </c>
       <c r="E168" t="n">
-        <v>0.10356690734624863</v>
+        <v>0.06442520767450333</v>
       </c>
       <c r="F168" t="n">
         <v>4.0</v>
@@ -3098,13 +3048,13 @@
         <v>4.0</v>
       </c>
       <c r="C169" t="n">
-        <v>0.3747617304325104</v>
+        <v>0.23312565684318542</v>
       </c>
       <c r="D169" t="n">
         <v>261.9456724917965</v>
       </c>
       <c r="E169" t="n">
-        <v>0.3024876117706299</v>
+        <v>0.1881665587425232</v>
       </c>
       <c r="F169" t="n">
         <v>3.0</v>
@@ -3118,13 +3068,13 @@
         <v>1.0</v>
       </c>
       <c r="C170" t="n">
-        <v>0.3985292911529541</v>
+        <v>0.24791058897972107</v>
       </c>
       <c r="D170" t="n">
         <v>261.9136333683507</v>
       </c>
       <c r="E170" t="n">
-        <v>0.0677696168422699</v>
+        <v>0.04215701296925545</v>
       </c>
       <c r="F170" t="n">
         <v>3.0</v>
@@ -3138,13 +3088,13 @@
         <v>6.0</v>
       </c>
       <c r="C171" t="n">
-        <v>0.6999629139900208</v>
+        <v>0.43542152643203735</v>
       </c>
       <c r="D171" t="n">
         <v>261.8009810208278</v>
       </c>
       <c r="E171" t="n">
-        <v>0.30655360221862793</v>
+        <v>0.1906958520412445</v>
       </c>
       <c r="F171" t="n">
         <v>3.0</v>
@@ -3158,13 +3108,13 @@
         <v>1.0</v>
       </c>
       <c r="C172" t="n">
-        <v>0.559756338596344</v>
+        <v>0.3482040762901306</v>
       </c>
       <c r="D172" t="n">
         <v>261.832411431518</v>
       </c>
       <c r="E172" t="n">
-        <v>0.1469498574733734</v>
+        <v>0.09141216427087784</v>
       </c>
       <c r="F172" t="n">
         <v>6.0</v>
@@ -3178,13 +3128,13 @@
         <v>8.0</v>
       </c>
       <c r="C173" t="n">
-        <v>0.4411461353302002</v>
+        <v>0.27442097663879395</v>
       </c>
       <c r="D173" t="n">
         <v>261.84218775469515</v>
       </c>
       <c r="E173" t="n">
-        <v>0.1697424352169037</v>
+        <v>0.10559060424566269</v>
       </c>
       <c r="F173" t="n">
         <v>5.0</v>
@@ -3198,13 +3148,13 @@
         <v>12.0</v>
       </c>
       <c r="C174" t="n">
-        <v>0.4147675037384033</v>
+        <v>0.2580117881298065</v>
       </c>
       <c r="D174" t="n">
         <v>261.8742012620678</v>
       </c>
       <c r="E174" t="n">
-        <v>0.0824146419763565</v>
+        <v>0.05126715451478958</v>
       </c>
       <c r="F174" t="n">
         <v>6.0</v>
@@ -3218,13 +3168,13 @@
         <v>2.0</v>
       </c>
       <c r="C175" t="n">
-        <v>0.2931596636772156</v>
+        <v>0.18236397206783295</v>
       </c>
       <c r="D175" t="n">
         <v>261.9081444294253</v>
       </c>
       <c r="E175" t="n">
-        <v>0.129132941365242</v>
+        <v>0.08032890409231186</v>
       </c>
       <c r="F175" t="n">
         <v>4.0</v>
@@ -3238,13 +3188,13 @@
         <v>4.0</v>
       </c>
       <c r="C176" t="n">
-        <v>0.3815269470214844</v>
+        <v>0.23733405768871307</v>
       </c>
       <c r="D176" t="n">
         <v>261.85269539989224</v>
       </c>
       <c r="E176" t="n">
-        <v>0.1205088198184967</v>
+        <v>0.07496415823698044</v>
       </c>
       <c r="F176" t="n">
         <v>3.0</v>
@@ -3258,13 +3208,13 @@
         <v>10.0</v>
       </c>
       <c r="C177" t="n">
-        <v>0.6677214503288269</v>
+        <v>0.4153652489185333</v>
       </c>
       <c r="D177" t="n">
         <v>261.73523225362436</v>
       </c>
       <c r="E177" t="n">
-        <v>0.47716882824897766</v>
+        <v>0.29682937264442444</v>
       </c>
       <c r="F177" t="n">
         <v>6.0</v>
@@ -3278,13 +3228,13 @@
         <v>10.0</v>
       </c>
       <c r="C178" t="n">
-        <v>0.833429753780365</v>
+        <v>0.5184463858604431</v>
       </c>
       <c r="D178" t="n">
         <v>261.64456146410316</v>
       </c>
       <c r="E178" t="n">
-        <v>0.19035542011260986</v>
+        <v>0.11841318756341934</v>
       </c>
       <c r="F178" t="n">
         <v>6.0</v>
@@ -3298,13 +3248,13 @@
         <v>10.0</v>
       </c>
       <c r="C179" t="n">
-        <v>0.8602044582366943</v>
+        <v>0.5351018905639648</v>
       </c>
       <c r="D179" t="n">
         <v>261.6337953543354</v>
       </c>
       <c r="E179" t="n">
-        <v>0.028472568839788437</v>
+        <v>0.01771175116300583</v>
       </c>
       <c r="F179" t="n">
         <v>6.0</v>
@@ -3318,13 +3268,13 @@
         <v>10.0</v>
       </c>
       <c r="C180" t="n">
-        <v>0.9158056378364563</v>
+        <v>0.5696893930435181</v>
       </c>
       <c r="D180" t="n">
         <v>261.62780508586667</v>
       </c>
       <c r="E180" t="n">
-        <v>0.11803000420331955</v>
+        <v>0.07342217862606049</v>
       </c>
       <c r="F180" t="n">
         <v>6.0</v>
@@ -3338,13 +3288,13 @@
         <v>10.0</v>
       </c>
       <c r="C181" t="n">
-        <v>0.9511350989341736</v>
+        <v>0.591666579246521</v>
       </c>
       <c r="D181" t="n">
         <v>261.6143715155233</v>
       </c>
       <c r="E181" t="n">
-        <v>0.03647772595286369</v>
+        <v>0.02269146777689457</v>
       </c>
       <c r="F181" t="n">
         <v>6.0</v>
@@ -3358,13 +3308,13 @@
         <v>10.0</v>
       </c>
       <c r="C182" t="n">
-        <v>1.073432445526123</v>
+        <v>0.6677433252334595</v>
       </c>
       <c r="D182" t="n">
         <v>261.6266045710891</v>
       </c>
       <c r="E182" t="n">
-        <v>0.26614075899124146</v>
+        <v>0.16555650532245636</v>
       </c>
       <c r="F182" t="n">
         <v>6.0</v>
@@ -3378,13 +3328,13 @@
         <v>4.0</v>
       </c>
       <c r="C183" t="n">
-        <v>0.5690993070602417</v>
+        <v>0.3540160059928894</v>
       </c>
       <c r="D183" t="n">
         <v>261.8092385280714</v>
       </c>
       <c r="E183" t="n">
-        <v>0.5048531293869019</v>
+        <v>0.3140507936477661</v>
       </c>
       <c r="F183" t="n">
         <v>4.0</v>
@@ -3398,13 +3348,13 @@
         <v>1.0</v>
       </c>
       <c r="C184" t="n">
-        <v>0.4929746091365814</v>
+        <v>0.30666160583496094</v>
       </c>
       <c r="D184" t="n">
         <v>261.8645538790942</v>
       </c>
       <c r="E184" t="n">
-        <v>0.11575106531381607</v>
+        <v>0.0720045268535614</v>
       </c>
       <c r="F184" t="n">
         <v>4.0</v>
@@ -3418,13 +3368,13 @@
         <v>1.0</v>
       </c>
       <c r="C185" t="n">
-        <v>0.40551504492759705</v>
+        <v>0.2522561550140381</v>
       </c>
       <c r="D185" t="n">
         <v>261.86063939372787</v>
       </c>
       <c r="E185" t="n">
-        <v>0.14611230790615082</v>
+        <v>0.09089116007089615</v>
       </c>
       <c r="F185" t="n">
         <v>6.0</v>
@@ -3438,13 +3388,13 @@
         <v>5.0</v>
       </c>
       <c r="C186" t="n">
-        <v>0.26619550585746765</v>
+        <v>0.1655905395746231</v>
       </c>
       <c r="D186" t="n">
         <v>261.9041240218826</v>
       </c>
       <c r="E186" t="n">
-        <v>0.1610601395368576</v>
+        <v>0.10018965601921082</v>
       </c>
       <c r="F186" t="n">
         <v>3.0</v>
@@ -3458,13 +3408,13 @@
         <v>4.0</v>
       </c>
       <c r="C187" t="n">
-        <v>0.24060335755348206</v>
+        <v>0.14967060089111328</v>
       </c>
       <c r="D187" t="n">
         <v>261.9164291959897</v>
       </c>
       <c r="E187" t="n">
-        <v>0.025917239487171173</v>
+        <v>0.01612217165529728</v>
       </c>
       <c r="F187" t="n">
         <v>3.0</v>
@@ -3484,42 +3434,42 @@
         <v>262.025968659323</v>
       </c>
       <c r="E188" t="n">
-        <v>0.24060335755348206</v>
+        <v>0.14967060089111328</v>
       </c>
       <c r="F188" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="189">
-      <c r="A189" t="s" s="19">
+      <c r="A189" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="B189" s="19" t="n">
+      <c r="B189" s="7" t="n">
         <f>SUM(B167:B188)</f>
         <v>116.0</v>
       </c>
-      <c r="E189" s="19" t="n">
+      <c r="E189" s="7" t="n">
         <f>SUM(E167:E188)</f>
-        <v>3.740068979561329</v>
+        <v>2.326560989022255</v>
       </c>
     </row>
     <row r="190"/>
     <row r="191"/>
     <row r="192"/>
     <row r="193">
-      <c r="A193" t="s" s="19">
+      <c r="A193" t="s" s="7">
         <v>16</v>
       </c>
       <c r="B193" t="n">
         <v>-1.0</v>
       </c>
-      <c r="C193" t="s" s="19">
+      <c r="C193" t="s" s="7">
         <v>17</v>
       </c>
       <c r="D193" t="n">
         <v>-80.046878</v>
       </c>
-      <c r="E193" t="s" s="19">
+      <c r="E193" t="s" s="7">
         <v>18</v>
       </c>
       <c r="F193" t="n">
@@ -3527,37 +3477,37 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" t="s" s="19">
+      <c r="A194" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="B194" t="n" s="19">
+      <c r="B194" t="n" s="7">
         <v>5.0</v>
       </c>
-      <c r="C194" t="s" s="19">
+      <c r="C194" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="D194" t="n" s="20">
+      <c r="D194" t="n" s="8">
         <v>-1.0</v>
       </c>
     </row>
     <row r="195">
-      <c r="A195" t="s" s="19">
+      <c r="A195" t="s" s="7">
         <v>21</v>
       </c>
-      <c r="B195" t="n" s="20">
-        <v>3.6056344509124756</v>
-      </c>
-      <c r="C195" t="s" s="19">
+      <c r="B195" t="n" s="8">
+        <v>2.242934226989746</v>
+      </c>
+      <c r="C195" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="D195" t="n" s="20">
-        <v>340.0</v>
-      </c>
-      <c r="E195" t="s" s="19">
+      <c r="D195" t="n" s="8">
+        <v>333.0</v>
+      </c>
+      <c r="E195" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="F195" t="n" s="20">
-        <v>3.6056344509124756</v>
+      <c r="F195" t="n" s="8">
+        <v>2.242934226989746</v>
       </c>
     </row>
     <row r="196"/>
@@ -3609,13 +3559,13 @@
         <v>1.0</v>
       </c>
       <c r="C199" t="n">
-        <v>0.40551504492759705</v>
+        <v>0.2522561550140381</v>
       </c>
       <c r="D199" t="n">
         <v>261.86063939372787</v>
       </c>
       <c r="E199" t="n">
-        <v>0.40551504492759705</v>
+        <v>0.2522561550140381</v>
       </c>
       <c r="F199" t="n">
         <v>6.0</v>
@@ -3629,13 +3579,13 @@
         <v>1.0</v>
       </c>
       <c r="C200" t="n">
-        <v>0.4929746091365814</v>
+        <v>0.30666160583496094</v>
       </c>
       <c r="D200" t="n">
         <v>261.8645538790942</v>
       </c>
       <c r="E200" t="n">
-        <v>0.14611230790615082</v>
+        <v>0.09089116007089615</v>
       </c>
       <c r="F200" t="n">
         <v>4.0</v>
@@ -3649,13 +3599,13 @@
         <v>4.0</v>
       </c>
       <c r="C201" t="n">
-        <v>0.5690993070602417</v>
+        <v>0.3540160059928894</v>
       </c>
       <c r="D201" t="n">
         <v>261.8092385280714</v>
       </c>
       <c r="E201" t="n">
-        <v>0.11575106531381607</v>
+        <v>0.0720045268535614</v>
       </c>
       <c r="F201" t="n">
         <v>4.0</v>
@@ -3669,13 +3619,13 @@
         <v>1.0</v>
       </c>
       <c r="C202" t="n">
-        <v>0.6471188068389893</v>
+        <v>0.4025490880012512</v>
       </c>
       <c r="D202" t="n">
         <v>261.8530329755303</v>
       </c>
       <c r="E202" t="n">
-        <v>0.21096783876419067</v>
+        <v>0.13123542070388794</v>
       </c>
       <c r="F202" t="n">
         <v>3.0</v>
@@ -3689,13 +3639,13 @@
         <v>10.0</v>
       </c>
       <c r="C203" t="n">
-        <v>1.073432445526123</v>
+        <v>0.6677433252334595</v>
       </c>
       <c r="D203" t="n">
         <v>261.6266045710891</v>
       </c>
       <c r="E203" t="n">
-        <v>0.49173110723495483</v>
+        <v>0.3058880567550659</v>
       </c>
       <c r="F203" t="n">
         <v>6.0</v>
@@ -3709,13 +3659,13 @@
         <v>8.0</v>
       </c>
       <c r="C204" t="n">
-        <v>0.9836602210998535</v>
+        <v>0.6118992567062378</v>
       </c>
       <c r="D204" t="n">
         <v>261.6216537846275</v>
       </c>
       <c r="E204" t="n">
-        <v>0.16966231167316437</v>
+        <v>0.10554075241088867</v>
       </c>
       <c r="F204" t="n">
         <v>3.0</v>
@@ -3729,13 +3679,13 @@
         <v>5.0</v>
       </c>
       <c r="C205" t="n">
-        <v>1.1121973991394043</v>
+        <v>0.6918575763702393</v>
       </c>
       <c r="D205" t="n">
         <v>261.55286056275264</v>
       </c>
       <c r="E205" t="n">
-        <v>0.1432289034128189</v>
+        <v>0.08909749239683151</v>
       </c>
       <c r="F205" t="n">
         <v>3.0</v>
@@ -3749,13 +3699,13 @@
         <v>10.0</v>
       </c>
       <c r="C206" t="n">
-        <v>0.9511350989341736</v>
+        <v>0.591666579246521</v>
       </c>
       <c r="D206" t="n">
         <v>261.6143715155233</v>
       </c>
       <c r="E206" t="n">
-        <v>0.16477824747562408</v>
+        <v>0.10250256210565567</v>
       </c>
       <c r="F206" t="n">
         <v>6.0</v>
@@ -3769,13 +3719,13 @@
         <v>10.0</v>
       </c>
       <c r="C207" t="n">
-        <v>0.9158056378364563</v>
+        <v>0.5696893930435181</v>
       </c>
       <c r="D207" t="n">
         <v>261.62780508586667</v>
       </c>
       <c r="E207" t="n">
-        <v>0.03647772595286369</v>
+        <v>0.02269146777689457</v>
       </c>
       <c r="F207" t="n">
         <v>6.0</v>
@@ -3789,13 +3739,13 @@
         <v>10.0</v>
       </c>
       <c r="C208" t="n">
-        <v>0.8602044582366943</v>
+        <v>0.5351018905639648</v>
       </c>
       <c r="D208" t="n">
         <v>261.6337953543354</v>
       </c>
       <c r="E208" t="n">
-        <v>0.11803000420331955</v>
+        <v>0.07342217862606049</v>
       </c>
       <c r="F208" t="n">
         <v>6.0</v>
@@ -3809,13 +3759,13 @@
         <v>10.0</v>
       </c>
       <c r="C209" t="n">
-        <v>0.833429753780365</v>
+        <v>0.5184463858604431</v>
       </c>
       <c r="D209" t="n">
         <v>261.64456146410316</v>
       </c>
       <c r="E209" t="n">
-        <v>0.028472568839788437</v>
+        <v>0.01771175116300583</v>
       </c>
       <c r="F209" t="n">
         <v>6.0</v>
@@ -3829,13 +3779,13 @@
         <v>10.0</v>
       </c>
       <c r="C210" t="n">
-        <v>0.6677214503288269</v>
+        <v>0.4153652489185333</v>
       </c>
       <c r="D210" t="n">
         <v>261.73523225362436</v>
       </c>
       <c r="E210" t="n">
-        <v>0.19035542011260986</v>
+        <v>0.11841318756341934</v>
       </c>
       <c r="F210" t="n">
         <v>6.0</v>
@@ -3849,13 +3799,13 @@
         <v>1.0</v>
       </c>
       <c r="C211" t="n">
-        <v>0.48756301403045654</v>
+        <v>0.30329522490501404</v>
       </c>
       <c r="D211" t="n">
         <v>261.79625441958456</v>
       </c>
       <c r="E211" t="n">
-        <v>0.22453835606575012</v>
+        <v>0.13967715203762054</v>
       </c>
       <c r="F211" t="n">
         <v>3.0</v>
@@ -3869,13 +3819,13 @@
         <v>1.0</v>
       </c>
       <c r="C212" t="n">
-        <v>0.559756338596344</v>
+        <v>0.3482040762901306</v>
       </c>
       <c r="D212" t="n">
         <v>261.832411431518</v>
       </c>
       <c r="E212" t="n">
-        <v>0.49370869994163513</v>
+        <v>0.3071182370185852</v>
       </c>
       <c r="F212" t="n">
         <v>6.0</v>
@@ -3889,13 +3839,13 @@
         <v>12.0</v>
       </c>
       <c r="C213" t="n">
-        <v>0.4147675037384033</v>
+        <v>0.2580117881298065</v>
       </c>
       <c r="D213" t="n">
         <v>261.8742012620678</v>
       </c>
       <c r="E213" t="n">
-        <v>0.14805088937282562</v>
+        <v>0.09209708124399185</v>
       </c>
       <c r="F213" t="n">
         <v>6.0</v>
@@ -3909,13 +3859,13 @@
         <v>2.0</v>
       </c>
       <c r="C214" t="n">
-        <v>0.2931596636772156</v>
+        <v>0.18236397206783295</v>
       </c>
       <c r="D214" t="n">
         <v>261.9081444294253</v>
       </c>
       <c r="E214" t="n">
-        <v>0.129132941365242</v>
+        <v>0.08032890409231186</v>
       </c>
       <c r="F214" t="n">
         <v>4.0</v>
@@ -3929,13 +3879,13 @@
         <v>4.0</v>
       </c>
       <c r="C215" t="n">
-        <v>0.12855416536331177</v>
+        <v>0.0799688771367073</v>
       </c>
       <c r="D215" t="n">
         <v>262.02842904452655</v>
       </c>
       <c r="E215" t="n">
-        <v>0.25213780999183655</v>
+        <v>0.15684577822685242</v>
       </c>
       <c r="F215" t="n">
         <v>3.0</v>
@@ -3949,13 +3899,13 @@
         <v>3.0</v>
       </c>
       <c r="C216" t="n">
-        <v>0.10356690734624863</v>
+        <v>0.06442520767450333</v>
       </c>
       <c r="D216" t="n">
         <v>262.03744350084025</v>
       </c>
       <c r="E216" t="n">
-        <v>0.03341617435216904</v>
+        <v>0.020786987617611885</v>
       </c>
       <c r="F216" t="n">
         <v>4.0</v>
@@ -3975,23 +3925,23 @@
         <v>262.025968659323</v>
       </c>
       <c r="E217" t="n">
-        <v>0.10356690734624863</v>
+        <v>0.06442520767450333</v>
       </c>
       <c r="F217" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="218">
-      <c r="A218" t="s" s="19">
+      <c r="A218" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="B218" s="19" t="n">
+      <c r="B218" s="7" t="n">
         <f>SUM(B198:B217)</f>
         <v>103.0</v>
       </c>
-      <c r="E218" s="19" t="n">
+      <c r="E218" s="7" t="n">
         <f>SUM(E198:E217)</f>
-        <v>3.6056343242526054</v>
+        <v>2.2429340593516827</v>
       </c>
     </row>
   </sheetData>

</xml_diff>